<commit_message>
updating for an early game
</commit_message>
<xml_diff>
--- a/csv/soxpitch.xlsx
+++ b/csv/soxpitch.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="340">
   <si>
     <t>Season</t>
   </si>
@@ -985,6 +985,60 @@
   </si>
   <si>
     <t>Miguel Gonzalez</t>
+  </si>
+  <si>
+    <t>GS - games started</t>
+  </si>
+  <si>
+    <t>CG - complete game</t>
+  </si>
+  <si>
+    <t>ShO - shutouts</t>
+  </si>
+  <si>
+    <t>SV - saves</t>
+  </si>
+  <si>
+    <t>BS - blown saves</t>
+  </si>
+  <si>
+    <t>G (games) / IP - innings pitched = avg innings pitched</t>
+  </si>
+  <si>
+    <t>BF/TBF - total batters faced</t>
+  </si>
+  <si>
+    <t>WP - wild pitches</t>
+  </si>
+  <si>
+    <t>BK - Balk</t>
+  </si>
+  <si>
+    <t>SO - strike outs</t>
+  </si>
+  <si>
+    <t>GB - ground balls</t>
+  </si>
+  <si>
+    <t>FB - fly balls</t>
+  </si>
+  <si>
+    <t>LD - line drives</t>
+  </si>
+  <si>
+    <t>IFFB - infleld fly balls</t>
+  </si>
+  <si>
+    <t>RS - run support average (per start)</t>
+  </si>
+  <si>
+    <t>AVG - opposing batting average?</t>
+  </si>
+  <si>
+    <t>WHIP - walks and hits per innings pitched</t>
+  </si>
+  <si>
+    <t>WPA - win probability added</t>
   </si>
 </sst>
 </file>
@@ -1003,12 +1057,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1023,9 +1083,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1357,10 +1419,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:KM16"/>
+  <dimension ref="A1:KM51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1650,55 +1713,55 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="V1" t="s">
@@ -1707,37 +1770,37 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="AI1" t="s">
@@ -1764,19 +1827,19 @@
       <c r="AP1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>44</v>
       </c>
       <c r="AT1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
       <c r="AV1" t="s">
@@ -1821,10 +1884,10 @@
       <c r="BI1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BK1" s="2" t="s">
         <v>62</v>
       </c>
       <c r="BL1" t="e">
@@ -10915,6 +10978,171 @@
       </c>
       <c r="KM16">
         <v>26.8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>